<commit_message>
Adding the new agents
</commit_message>
<xml_diff>
--- a/Accounts-Schedules/5th-settelment-Trainers.xlsx
+++ b/Accounts-Schedules/5th-settelment-Trainers.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
   <si>
     <t>Trainers</t>
   </si>
@@ -153,6 +153,33 @@
   </si>
   <si>
     <t>Trainer - Talabat</t>
+  </si>
+  <si>
+    <t>Monday, June 2</t>
+  </si>
+  <si>
+    <t>Tuesday, June 3</t>
+  </si>
+  <si>
+    <t>Tuesday, June 4</t>
+  </si>
+  <si>
+    <t>Tuesday, June 5</t>
+  </si>
+  <si>
+    <t>Friday, June 6</t>
+  </si>
+  <si>
+    <t>Saturday, June 7</t>
+  </si>
+  <si>
+    <t>Sunday, June 8</t>
+  </si>
+  <si>
+    <t>Ahmed Hafiz</t>
+  </si>
+  <si>
+    <t>Training Manager</t>
   </si>
 </sst>
 </file>
@@ -1116,7 +1143,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1222,8 +1249,53 @@
     <xf numFmtId="179" fontId="14" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="179" fontId="14" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="179" fontId="14" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="179" fontId="12" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
@@ -1764,10 +1836,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:E17"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -1778,7 +1850,7 @@
     <col min="15" max="15" width="9.45454545454546"/>
   </cols>
   <sheetData>
-    <row r="1" ht="23" customHeight="1" spans="1:1">
+    <row r="1" ht="23.75" customHeight="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1962,7 +2034,7 @@
       </c>
     </row>
     <row r="8" ht="15.25" spans="17:17">
-      <c r="Q8" s="37"/>
+      <c r="Q8" s="52"/>
     </row>
     <row r="9" ht="15.25" spans="1:17">
       <c r="A9" s="8" t="s">
@@ -2131,35 +2203,36 @@
       <c r="H13" s="23">
         <v>0.333333333333333</v>
       </c>
-      <c r="I13" s="35">
+      <c r="I13" s="49">
         <v>0.708333333333333</v>
       </c>
       <c r="J13" s="23">
         <v>0.333333333333333</v>
       </c>
-      <c r="K13" s="35">
+      <c r="K13" s="49">
         <v>0.708333333333333</v>
       </c>
       <c r="L13" s="23">
         <v>0.458333333333333</v>
       </c>
-      <c r="M13" s="35">
+      <c r="M13" s="49">
         <v>0.833333333333333</v>
       </c>
       <c r="N13" s="23">
         <v>0.458333333333333</v>
       </c>
-      <c r="O13" s="35">
+      <c r="O13" s="49">
         <v>0.833333333333333</v>
       </c>
       <c r="P13" s="23">
         <v>0.458333333333333</v>
       </c>
-      <c r="Q13" s="35">
+      <c r="Q13" s="49">
         <v>0.833333333333333</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="14" ht="15.25"/>
+    <row r="15" ht="15.25" spans="1:15">
       <c r="A15" s="24" t="s">
         <v>28</v>
       </c>
@@ -2196,7 +2269,7 @@
       </c>
       <c r="O15" s="27"/>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" ht="15.25" spans="1:15">
       <c r="A16" s="28"/>
       <c r="B16" s="29"/>
       <c r="C16" s="29"/>
@@ -2233,7 +2306,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" ht="15.25" spans="1:15">
       <c r="A17" s="31">
         <v>10259455</v>
       </c>
@@ -2267,10 +2340,10 @@
       <c r="K17" s="34">
         <v>0.833333333333333</v>
       </c>
-      <c r="L17" s="36" t="s">
+      <c r="L17" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="M17" s="36" t="s">
+      <c r="M17" s="50" t="s">
         <v>27</v>
       </c>
       <c r="N17" s="34">
@@ -2280,8 +2353,176 @@
         <v>0.833333333333333</v>
       </c>
     </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="37"/>
+      <c r="F19" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="K19" s="38"/>
+      <c r="L19" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="M19" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="N19" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="O19" s="38"/>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="39"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="I20" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="J20" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="K20" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="L20" s="40"/>
+      <c r="M20" s="40"/>
+      <c r="N20" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="O20" s="41" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="42">
+        <v>10210885</v>
+      </c>
+      <c r="B21" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="45">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E21" s="45">
+        <v>0.75</v>
+      </c>
+      <c r="F21" s="45">
+        <v>0.375</v>
+      </c>
+      <c r="G21" s="45">
+        <v>0.75</v>
+      </c>
+      <c r="H21" s="45">
+        <v>0.375</v>
+      </c>
+      <c r="I21" s="45">
+        <v>0.75</v>
+      </c>
+      <c r="J21" s="45">
+        <v>0.5</v>
+      </c>
+      <c r="K21" s="45">
+        <v>0.875</v>
+      </c>
+      <c r="L21" s="45">
+        <v>0.5</v>
+      </c>
+      <c r="M21" s="45">
+        <v>0.875</v>
+      </c>
+      <c r="N21" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="O21" s="51" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="46">
+        <v>10259455</v>
+      </c>
+      <c r="B22" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="48">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="E22" s="48">
+        <v>0.833333333333333</v>
+      </c>
+      <c r="F22" s="48">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="G22" s="48">
+        <v>0.833333333333333</v>
+      </c>
+      <c r="H22" s="48">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="I22" s="48">
+        <v>0.833333333333333</v>
+      </c>
+      <c r="J22" s="48">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="K22" s="48">
+        <v>0.833333333333333</v>
+      </c>
+      <c r="L22" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="M22" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="N22" s="48">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="O22" s="48">
+        <v>0.833333333333333</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="41">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
@@ -2307,11 +2548,21 @@
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="J15:K15"/>
     <mergeCell ref="N15:O15"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="N19:O19"/>
     <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A19:A20"/>
     <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B19:B20"/>
     <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C19:C20"/>
     <mergeCell ref="L15:L16"/>
+    <mergeCell ref="L19:L20"/>
     <mergeCell ref="M15:M16"/>
+    <mergeCell ref="M19:M20"/>
     <mergeCell ref="A9:B10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>